<commit_message>
alvenaria estrutural - cargas horizontais de vento - parte 1
</commit_message>
<xml_diff>
--- a/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
+++ b/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casa\Dropbox\Curso Alvenaria Estrutural engenhaBIM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" tabRatio="779"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="779"/>
   </bookViews>
   <sheets>
     <sheet name="Tensões Vento e Desaprumo" sheetId="18" r:id="rId1"/>
@@ -195,12 +190,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -336,17 +331,17 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyAlignment="1">
@@ -357,21 +352,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -381,30 +376,30 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -702,7 +697,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -712,51 +707,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="52.9296875" customWidth="1"/>
-    <col min="14" max="14" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="53" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-    </row>
-    <row r="2" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-    </row>
-    <row r="3" spans="1:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -771,7 +767,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -789,7 +785,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="20" t="s">
         <v>1</v>
       </c>
@@ -825,7 +821,7 @@
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -872,7 +868,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -913,7 +909,7 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
         <v>3</v>
       </c>
@@ -961,7 +957,7 @@
         <v>2.3570226039551587E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -1002,7 +998,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -1049,7 +1045,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -1097,7 +1093,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1117,7 +1113,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1137,7 +1133,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1156,7 +1152,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -1176,7 +1172,7 @@
         <v>158.30266666666665</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>1</v>
       </c>
@@ -1219,7 +1215,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="3">
         <v>5</v>
       </c>
@@ -1266,7 +1262,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
         <v>4</v>
       </c>
@@ -1313,7 +1309,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="3">
         <v>3</v>
       </c>
@@ -1361,7 +1357,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="3">
         <v>2</v>
       </c>
@@ -1408,7 +1404,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="3">
         <v>1</v>
       </c>
@@ -1455,7 +1451,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
@@ -1502,7 +1498,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="M24" s="23">
         <f>M22+M19+M16</f>
         <v>4101.04</v>
@@ -1524,48 +1520,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="17" customWidth="1"/>
-    <col min="2" max="2" width="10.73046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.73046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.3984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.265625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="9.1328125" style="6"/>
-    <col min="9" max="9" width="10.73046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.86328125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="12.265625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="12.73046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.59765625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.1328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="6"/>
+    <col min="9" max="9" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.59765625" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.73046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.3984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.1328125" style="6"/>
+    <col min="17" max="17" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="14.25" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
         <v>49</v>
       </c>
@@ -1583,7 +1579,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>18</v>
       </c>
@@ -1609,7 +1605,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>0</v>
       </c>
@@ -1635,7 +1631,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="19">
         <v>1</v>
       </c>
@@ -1661,7 +1657,7 @@
         <v>-1998.7949999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="19">
         <f>A5+1</f>
         <v>2</v>
@@ -1688,7 +1684,7 @@
         <v>-1085.6880000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="19">
         <f t="shared" ref="A7:A14" si="2">A6+1</f>
         <v>3</v>
@@ -1711,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A8" s="19">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -1734,7 +1730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A9" s="19">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -1757,7 +1753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A10" s="19">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -1780,7 +1776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A11" s="19">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -1803,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A12" s="19">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -1826,7 +1822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A13" s="19">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -1849,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A14" s="19">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -1872,7 +1868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="I15" s="28">
         <f>F5</f>
         <v>3951.4519999999993</v>
@@ -1888,7 +1884,7 @@
         <v>11289.862857142856</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
       <c r="C17" s="6" t="s">
         <v>12</v>
       </c>
@@ -1906,13 +1902,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
       <c r="E18" s="6">
         <f>1-(20/40)^3</f>
         <v>0.875</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D20" s="6">
         <f>2.8/0.14</f>
         <v>19.999999999999996</v>
@@ -1921,7 +1917,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
alvenaria estrutural - cargas orizontais de vento - parte 1
</commit_message>
<xml_diff>
--- a/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
+++ b/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Tensões Vento e Desaprumo" sheetId="18" r:id="rId1"/>
     <sheet name="Flexo-Compressão" sheetId="22" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>Parede</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Ft (kn/m)</t>
+  </si>
+  <si>
+    <t>NBR 6123/1988</t>
   </si>
 </sst>
 </file>
@@ -256,7 +259,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +280,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,7 +344,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -392,14 +401,17 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -697,7 +709,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -707,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,32 +737,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
@@ -785,7 +797,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>1</v>
       </c>
@@ -819,9 +831,11 @@
       <c r="K5" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="L5" s="33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1512,7 +1526,7 @@
     <mergeCell ref="A1:K2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1550,15 +1564,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:10" thickTop="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
alvenaria estrutural - carga horizontal de vento parte 2
</commit_message>
<xml_diff>
--- a/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
+++ b/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>Parede</t>
   </si>
@@ -106,12 +106,6 @@
     <t>Térreo</t>
   </si>
   <si>
-    <t>cat IV</t>
-  </si>
-  <si>
-    <t>classe B</t>
-  </si>
-  <si>
     <t>Fv (Kn/m)</t>
   </si>
   <si>
@@ -188,6 +182,15 @@
   </si>
   <si>
     <t>NBR 6123/1988</t>
+  </si>
+  <si>
+    <t>Cat. IV</t>
+  </si>
+  <si>
+    <t>Classe B</t>
+  </si>
+  <si>
+    <t>Tabela 2</t>
   </si>
 </sst>
 </file>
@@ -200,7 +203,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +257,36 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -344,7 +377,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -401,17 +434,20 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -719,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,27 +767,27 @@
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="53" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -764,12 +800,12 @@
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>28</v>
+      <c r="E3" s="34" t="s">
+        <v>54</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -786,8 +822,8 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>29</v>
+      <c r="E4" s="34" t="s">
+        <v>55</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -823,16 +859,16 @@
         <v>7</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="L5" s="33" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -876,7 +912,7 @@
       </c>
       <c r="L6" s="1"/>
       <c r="M6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N6" s="21">
         <v>18</v>
@@ -964,7 +1000,7 @@
       </c>
       <c r="L8" s="1"/>
       <c r="M8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N8" s="22">
         <f>1/(100*SQRT(N6))</f>
@@ -1056,7 +1092,7 @@
         <v>2423</v>
       </c>
       <c r="N10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1104,15 +1140,17 @@
         <v>403.83333333333331</v>
       </c>
       <c r="N11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="33" t="s">
+        <v>56</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1124,10 +1162,10 @@
         <v>2.8</v>
       </c>
       <c r="N12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1144,7 +1182,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="N13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
@@ -1163,7 +1201,7 @@
         <v>15</v>
       </c>
       <c r="N14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1215,10 +1253,10 @@
         <v>8</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="25">
@@ -1226,7 +1264,7 @@
         <v>2374.54</v>
       </c>
       <c r="N16" s="24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
@@ -1273,7 +1311,7 @@
         <v>99</v>
       </c>
       <c r="N17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
@@ -1320,7 +1358,7 @@
         <v>2.5</v>
       </c>
       <c r="N18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
@@ -1368,7 +1406,7 @@
         <v>247.5</v>
       </c>
       <c r="N19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
@@ -1415,7 +1453,7 @@
         <v>493</v>
       </c>
       <c r="N20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
@@ -1462,7 +1500,7 @@
         <v>3</v>
       </c>
       <c r="N21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1509,7 +1547,7 @@
         <v>1479</v>
       </c>
       <c r="N22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
@@ -1518,7 +1556,7 @@
         <v>4101.04</v>
       </c>
       <c r="N24" s="23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1564,20 +1602,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:10" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="6" t="s">
@@ -1903,17 +1941,17 @@
         <v>12</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J17" s="28">
         <f>J16/1000</f>
         <v>11.289862857142856</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
@@ -1928,15 +1966,15 @@
         <v>19.999999999999996</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alvenaria estrutural - cargas horizontais de vento - parte 3
</commit_message>
<xml_diff>
--- a/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
+++ b/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
   <si>
     <t>Parede</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>Tabela 2</t>
+  </si>
+  <si>
+    <t>qv * altura</t>
   </si>
 </sst>
 </file>
@@ -377,7 +380,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -448,6 +451,9 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -755,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,7 +901,7 @@
         <v>36.4</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" ref="H6:H11" si="1">(0.613*(G6^2))/1000</f>
+        <f>(0.613*(G6^2))/1000</f>
         <v>0.81220047999999989</v>
       </c>
       <c r="I6" s="2">
@@ -903,11 +909,11 @@
         <v>1.2183007199999998</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" ref="J6:J11" si="2">(4100*$N$8)/23.7</f>
+        <f t="shared" ref="J6:J11" si="1">(4100*$N$8)/23.7</f>
         <v>0.40775496524118782</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" ref="K6:K11" si="3">I6+J6</f>
+        <f t="shared" ref="K6:K11" si="2">I6+J6</f>
         <v>1.6260556852411876</v>
       </c>
       <c r="L6" s="1"/>
@@ -942,7 +948,7 @@
         <v>35.200000000000003</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H6:H11" si="3">(0.613*(G7^2))/1000</f>
         <v>0.75953152000000013</v>
       </c>
       <c r="I7" s="2">
@@ -950,11 +956,11 @@
         <v>2.2785945600000002</v>
       </c>
       <c r="J7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.40775496524118782</v>
+      </c>
+      <c r="K7" s="2">
         <f t="shared" si="2"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K7" s="2">
-        <f t="shared" si="3"/>
         <v>2.6863495252411882</v>
       </c>
       <c r="L7" s="1"/>
@@ -983,7 +989,7 @@
         <v>35.200000000000003</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.75953152000000013</v>
       </c>
       <c r="I8" s="2">
@@ -991,11 +997,11 @@
         <v>2.2785945600000002</v>
       </c>
       <c r="J8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.40775496524118782</v>
+      </c>
+      <c r="K8" s="2">
         <f t="shared" si="2"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K8" s="2">
-        <f t="shared" si="3"/>
         <v>2.6863495252411882</v>
       </c>
       <c r="L8" s="1"/>
@@ -1031,7 +1037,7 @@
         <v>33.199999999999996</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.67567311999999979</v>
       </c>
       <c r="I9" s="2">
@@ -1039,11 +1045,11 @@
         <v>2.0270193599999993</v>
       </c>
       <c r="J9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.40775496524118782</v>
+      </c>
+      <c r="K9" s="2">
         <f t="shared" si="2"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K9" s="2">
-        <f t="shared" si="3"/>
         <v>2.4347743252411869</v>
       </c>
       <c r="L9" s="1"/>
@@ -1072,7 +1078,7 @@
         <v>33.199999999999996</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.67567311999999979</v>
       </c>
       <c r="I10" s="2">
@@ -1080,11 +1086,11 @@
         <v>2.0270193599999993</v>
       </c>
       <c r="J10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.40775496524118782</v>
+      </c>
+      <c r="K10" s="2">
         <f t="shared" si="2"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K10" s="2">
-        <f t="shared" si="3"/>
         <v>2.4347743252411869</v>
       </c>
       <c r="L10" s="1"/>
@@ -1119,7 +1125,7 @@
         <v>30.4</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.56651008000000003</v>
       </c>
       <c r="I11" s="2">
@@ -1127,11 +1133,11 @@
         <v>1.6995302400000001</v>
       </c>
       <c r="J11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.40775496524118782</v>
+      </c>
+      <c r="K11" s="2">
         <f t="shared" si="2"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K11" s="2">
-        <f t="shared" si="3"/>
         <v>2.1072852052411877</v>
       </c>
       <c r="L11" s="1"/>
@@ -1154,7 +1160,9 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="I12" s="35" t="s">
+        <v>57</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>

</xml_diff>

<commit_message>
alvenaria estrutural - imperfeições globais (desaprumo)
</commit_message>
<xml_diff>
--- a/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
+++ b/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="82">
   <si>
     <t>Parede</t>
   </si>
@@ -109,51 +109,6 @@
     <t>Fv (Kn/m)</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>desprumo</t>
-  </si>
-  <si>
-    <t>comprimento total</t>
-  </si>
-  <si>
-    <t>comprimento por pavimento</t>
-  </si>
-  <si>
-    <t>altura da parede</t>
-  </si>
-  <si>
-    <t>kn/m3</t>
-  </si>
-  <si>
-    <t>espessura</t>
-  </si>
-  <si>
-    <t>peso próprio paredes</t>
-  </si>
-  <si>
-    <t>volume de piso</t>
-  </si>
-  <si>
-    <t>kn de piso/m3</t>
-  </si>
-  <si>
-    <t>kn de piso por pavimento</t>
-  </si>
-  <si>
-    <t>m2 de piso</t>
-  </si>
-  <si>
-    <t>kn/m2 de sobrecarga</t>
-  </si>
-  <si>
-    <t>kn de sobrecarga</t>
-  </si>
-  <si>
-    <t>kn</t>
-  </si>
-  <si>
     <t>Fd (Kn/m)</t>
   </si>
   <si>
@@ -194,19 +149,137 @@
   </si>
   <si>
     <t>qv * altura</t>
+  </si>
+  <si>
+    <t>NBR15812-1/2010</t>
+  </si>
+  <si>
+    <t>Altura (H)</t>
+  </si>
+  <si>
+    <t>Desprumo</t>
+  </si>
+  <si>
+    <t>Item 8.3.2.2 da NBR15812-1 (Imperfeições geométricas globais)</t>
+  </si>
+  <si>
+    <t>Comprimento de parede</t>
+  </si>
+  <si>
+    <t>Tabela revit</t>
+  </si>
+  <si>
+    <t>Comprimento por pavimento</t>
+  </si>
+  <si>
+    <t>Dividindo comprimento de parede por pavimento</t>
+  </si>
+  <si>
+    <t>Altura da parede</t>
+  </si>
+  <si>
+    <t>Espessura da parede</t>
+  </si>
+  <si>
+    <t>Kn/m³</t>
+  </si>
+  <si>
+    <t>Peso Próprio Paredes</t>
+  </si>
+  <si>
+    <t>Altura da parede em metros</t>
+  </si>
+  <si>
+    <t>Espessura da parede em metro</t>
+  </si>
+  <si>
+    <t>Peso da parede em kn</t>
+  </si>
+  <si>
+    <t>Metro cúbico de parede</t>
+  </si>
+  <si>
+    <t>Volume por pavimento (parede)</t>
+  </si>
+  <si>
+    <t>Volume de Piso</t>
+  </si>
+  <si>
+    <t>m² de Piso</t>
+  </si>
+  <si>
+    <t>Peso total</t>
+  </si>
+  <si>
+    <t>Volume disponível no Revit - vista 3D (em m³)</t>
+  </si>
+  <si>
+    <t>Basta clicar numa laje para o revit apresentar o volume (98.607 m³) - arredondamos</t>
+  </si>
+  <si>
+    <t>kN de piso por pavimento</t>
+  </si>
+  <si>
+    <t>KN/m² de sobrecarga</t>
+  </si>
+  <si>
+    <t>kN de sobrecarga</t>
+  </si>
+  <si>
+    <t>KN</t>
+  </si>
+  <si>
+    <t>KN de piso/m³</t>
+  </si>
+  <si>
+    <t>Valor do Kn por metro cúbico de piso</t>
+  </si>
+  <si>
+    <t>Kn total por piso (volume do piso * Kn por m³)</t>
+  </si>
+  <si>
+    <t>Peso próprio do piso (desconsiderando porta e outros equipamentos)</t>
+  </si>
+  <si>
+    <t>Peso próprio das paredes (desconsiderando alguns equipamentos)</t>
+  </si>
+  <si>
+    <t>Metros quadrados de piso</t>
+  </si>
+  <si>
+    <t>Basta clicar numa laje para o revit apresentar o área (493.037 m²) - arredondamos</t>
+  </si>
+  <si>
+    <t>Total de peso por pavimento em Kn</t>
+  </si>
+  <si>
+    <t>Volume de parede por pavimento</t>
+  </si>
+  <si>
+    <t>Peso do concreto armado</t>
+  </si>
+  <si>
+    <t>Sobrecarga de utilização</t>
+  </si>
+  <si>
+    <t>índice de 3 porque estamos considerando revestimento</t>
+  </si>
+  <si>
+    <t>KN cal. lado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,8 +367,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +410,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,7 +474,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -424,13 +518,6 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -454,6 +541,49 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -759,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,45 +903,47 @@
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27" style="32" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="61.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="34" t="s">
-        <v>54</v>
+      <c r="E3" s="29" t="s">
+        <v>39</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -821,15 +953,15 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="34" t="s">
-        <v>55</v>
+      <c r="E4" s="29" t="s">
+        <v>40</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -839,7 +971,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>1</v>
       </c>
@@ -868,16 +1000,16 @@
         <v>28</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="L5" s="32" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -909,22 +1041,24 @@
         <v>1.2183007199999998</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" ref="J6:J11" si="1">(4100*$N$8)/23.7</f>
-        <v>0.40775496524118782</v>
+        <f>(N24*$N$8)/23.7</f>
+        <v>0.40785839576895633</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" ref="K6:K11" si="2">I6+J6</f>
-        <v>1.6260556852411876</v>
-      </c>
-      <c r="L6" s="1"/>
-      <c r="M6" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="21">
+        <f t="shared" ref="K6:K11" si="1">I6+J6</f>
+        <v>1.6261591157689561</v>
+      </c>
+      <c r="L6" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="33">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -948,7 +1082,7 @@
         <v>35.200000000000003</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" ref="H6:H11" si="3">(0.613*(G7^2))/1000</f>
+        <f t="shared" ref="H6:H11" si="2">(0.613*(G7^2))/1000</f>
         <v>0.75953152000000013</v>
       </c>
       <c r="I7" s="2">
@@ -956,16 +1090,17 @@
         <v>2.2785945600000002</v>
       </c>
       <c r="J7" s="2">
+        <f>(N24*N8)/23.7</f>
+        <v>0.40785839576895633</v>
+      </c>
+      <c r="K7" s="2">
         <f t="shared" si="1"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K7" s="2">
-        <f t="shared" si="2"/>
-        <v>2.6863495252411882</v>
+        <v>2.6864529557689565</v>
       </c>
       <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="M7" s="37"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>3</v>
       </c>
@@ -989,31 +1124,34 @@
         <v>35.200000000000003</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.75953152000000013</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" ref="I8:I11" si="4">H8*3</f>
+        <f t="shared" ref="I8:I11" si="3">H8*3</f>
         <v>2.2785945600000002</v>
       </c>
       <c r="J8" s="2">
+        <f>(N24*$N$8)/23.7</f>
+        <v>0.40785839576895633</v>
+      </c>
+      <c r="K8" s="2">
         <f t="shared" si="1"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K8" s="2">
-        <f t="shared" si="2"/>
-        <v>2.6863495252411882</v>
+        <v>2.6864529557689565</v>
       </c>
       <c r="L8" s="1"/>
-      <c r="M8" t="s">
-        <v>30</v>
-      </c>
-      <c r="N8" s="22">
+      <c r="M8" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" s="34">
         <f>1/(100*SQRT(N6))</f>
         <v>2.3570226039551587E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="O8" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -1037,24 +1175,25 @@
         <v>33.199999999999996</v>
       </c>
       <c r="H9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.67567311999999979</v>
+      </c>
+      <c r="I9" s="2">
         <f t="shared" si="3"/>
-        <v>0.67567311999999979</v>
-      </c>
-      <c r="I9" s="2">
-        <f t="shared" si="4"/>
         <v>2.0270193599999993</v>
       </c>
       <c r="J9" s="2">
+        <f>(N24*$N$8)/23.7</f>
+        <v>0.40785839576895633</v>
+      </c>
+      <c r="K9" s="2">
         <f t="shared" si="1"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K9" s="2">
-        <f t="shared" si="2"/>
-        <v>2.4347743252411869</v>
+        <v>2.4348777557689556</v>
       </c>
       <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="M9" s="37"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -1078,7 +1217,7 @@
         <v>33.199999999999996</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.67567311999999979</v>
       </c>
       <c r="I10" s="2">
@@ -1086,22 +1225,25 @@
         <v>2.0270193599999993</v>
       </c>
       <c r="J10" s="2">
+        <f>(N24*$N$8)/23.7</f>
+        <v>0.40785839576895633</v>
+      </c>
+      <c r="K10" s="2">
         <f t="shared" si="1"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K10" s="2">
-        <f t="shared" si="2"/>
-        <v>2.4347743252411869</v>
+        <v>2.4348777557689556</v>
       </c>
       <c r="L10" s="1"/>
-      <c r="M10">
+      <c r="M10" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" s="32">
         <v>2423</v>
       </c>
-      <c r="N10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -1125,55 +1267,63 @@
         <v>30.4</v>
       </c>
       <c r="H11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.56651008000000003</v>
+      </c>
+      <c r="I11" s="2">
         <f t="shared" si="3"/>
-        <v>0.56651008000000003</v>
-      </c>
-      <c r="I11" s="2">
-        <f t="shared" si="4"/>
         <v>1.6995302400000001</v>
       </c>
       <c r="J11" s="2">
+        <f>(N24*$N$8)/23.7</f>
+        <v>0.40785839576895633</v>
+      </c>
+      <c r="K11" s="2">
         <f t="shared" si="1"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K11" s="2">
-        <f t="shared" si="2"/>
-        <v>2.1072852052411877</v>
+        <v>2.1073886357689564</v>
       </c>
       <c r="L11" s="1"/>
-      <c r="M11">
-        <f>M10/6</f>
+      <c r="M11" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" s="39">
+        <f>N10/6</f>
         <v>403.83333333333331</v>
       </c>
-      <c r="N11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="33" t="s">
-        <v>56</v>
+      <c r="E12" s="28" t="s">
+        <v>41</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="J12" s="1"/>
+      <c r="I12" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="45" t="s">
+        <v>81</v>
+      </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12">
+      <c r="M12" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="N12" s="32">
         <v>2.8</v>
       </c>
-      <c r="N12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1186,14 +1336,17 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13">
+      <c r="M13" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" s="32">
         <v>0.14000000000000001</v>
       </c>
-      <c r="N13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="O13" s="35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1205,14 +1358,17 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14">
+      <c r="M14" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14" s="32">
         <v>15</v>
       </c>
-      <c r="N14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -1227,12 +1383,21 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15">
-        <f>M11*M12*M13</f>
+      <c r="M15" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="N15" s="39">
+        <f>N11*N12*N13</f>
         <v>158.30266666666665</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="P15" s="35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>1</v>
       </c>
@@ -1261,21 +1426,27 @@
         <v>8</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="L16" s="1"/>
-      <c r="M16" s="25">
-        <f>M15*M14</f>
+      <c r="M16" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="N16" s="40">
+        <f>N14*N15</f>
         <v>2374.54</v>
       </c>
-      <c r="N16" s="24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="O16" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="P16" s="35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>5</v>
       </c>
@@ -1295,11 +1466,11 @@
         <v>1</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" ref="G17:G22" si="5">C17*D17*E17*F17</f>
+        <f t="shared" ref="G17:G22" si="4">C17*D17*E17*F17</f>
         <v>36.4</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" ref="H17:H22" si="6">(0.613*(G17^2))/1000</f>
+        <f t="shared" ref="H17:H22" si="5">(0.613*(G17^2))/1000</f>
         <v>0.81220047999999989</v>
       </c>
       <c r="I17" s="2">
@@ -1307,22 +1478,28 @@
         <v>1.2183007199999998</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" ref="J17:J22" si="7">(4100*$N$8)/23.7</f>
+        <f t="shared" ref="J17:J22" si="6">(4100*$N$8)/23.7</f>
         <v>0.40775496524118782</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" ref="K17:K22" si="8">I17+J17</f>
+        <f t="shared" ref="K17:K22" si="7">I17+J17</f>
         <v>1.6260556852411876</v>
       </c>
       <c r="L17" s="1"/>
-      <c r="M17">
+      <c r="M17" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="N17" s="32">
         <v>99</v>
       </c>
-      <c r="N17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="O17" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="P17" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>4</v>
       </c>
@@ -1342,11 +1519,11 @@
         <v>1</v>
       </c>
       <c r="G18" s="2">
+        <f t="shared" si="4"/>
+        <v>35.200000000000003</v>
+      </c>
+      <c r="H18" s="2">
         <f t="shared" si="5"/>
-        <v>35.200000000000003</v>
-      </c>
-      <c r="H18" s="2">
-        <f t="shared" si="6"/>
         <v>0.75953152000000013</v>
       </c>
       <c r="I18" s="2">
@@ -1354,22 +1531,28 @@
         <v>2.2785945600000002</v>
       </c>
       <c r="J18" s="2">
+        <f t="shared" si="6"/>
+        <v>0.40775496524118782</v>
+      </c>
+      <c r="K18" s="2">
         <f t="shared" si="7"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K18" s="2">
-        <f t="shared" si="8"/>
         <v>2.6863495252411882</v>
       </c>
       <c r="L18" s="1"/>
-      <c r="M18">
+      <c r="M18" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="N18" s="32">
         <v>2.5</v>
       </c>
-      <c r="N18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="O18" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="P18" s="35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>3</v>
       </c>
@@ -1389,35 +1572,41 @@
         <v>1</v>
       </c>
       <c r="G19" s="2">
+        <f t="shared" si="4"/>
+        <v>35.200000000000003</v>
+      </c>
+      <c r="H19" s="2">
         <f t="shared" si="5"/>
-        <v>35.200000000000003</v>
-      </c>
-      <c r="H19" s="2">
+        <v>0.75953152000000013</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" ref="I19:I22" si="8">H19*3</f>
+        <v>2.2785945600000002</v>
+      </c>
+      <c r="J19" s="2">
         <f t="shared" si="6"/>
-        <v>0.75953152000000013</v>
-      </c>
-      <c r="I19" s="2">
-        <f t="shared" ref="I19:I22" si="9">H19*3</f>
-        <v>2.2785945600000002</v>
-      </c>
-      <c r="J19" s="2">
+        <v>0.40775496524118782</v>
+      </c>
+      <c r="K19" s="2">
         <f t="shared" si="7"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K19" s="2">
-        <f t="shared" si="8"/>
         <v>2.6863495252411882</v>
       </c>
       <c r="L19" s="1"/>
-      <c r="M19" s="25">
-        <f>M17*M18</f>
+      <c r="M19" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="N19" s="42">
+        <f>N17*N18</f>
         <v>247.5</v>
       </c>
-      <c r="N19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="O19" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="P19" s="35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2</v>
       </c>
@@ -1437,34 +1626,40 @@
         <v>1</v>
       </c>
       <c r="G20" s="2">
+        <f t="shared" si="4"/>
+        <v>33.199999999999996</v>
+      </c>
+      <c r="H20" s="2">
         <f t="shared" si="5"/>
-        <v>33.199999999999996</v>
-      </c>
-      <c r="H20" s="2">
+        <v>0.67567311999999979</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="8"/>
+        <v>2.0270193599999993</v>
+      </c>
+      <c r="J20" s="2">
         <f t="shared" si="6"/>
-        <v>0.67567311999999979</v>
-      </c>
-      <c r="I20" s="2">
-        <f t="shared" si="9"/>
-        <v>2.0270193599999993</v>
-      </c>
-      <c r="J20" s="2">
+        <v>0.40775496524118782</v>
+      </c>
+      <c r="K20" s="2">
         <f t="shared" si="7"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K20" s="2">
-        <f t="shared" si="8"/>
         <v>2.4347743252411869</v>
       </c>
       <c r="L20" s="1"/>
-      <c r="M20">
+      <c r="M20" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="N20" s="32">
         <v>493</v>
       </c>
-      <c r="N20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="O20" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="P20" s="35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>1</v>
       </c>
@@ -1484,11 +1679,11 @@
         <v>1</v>
       </c>
       <c r="G21" s="2">
+        <f t="shared" si="4"/>
+        <v>33.199999999999996</v>
+      </c>
+      <c r="H21" s="2">
         <f t="shared" si="5"/>
-        <v>33.199999999999996</v>
-      </c>
-      <c r="H21" s="2">
-        <f t="shared" si="6"/>
         <v>0.67567311999999979</v>
       </c>
       <c r="I21" s="2">
@@ -1496,22 +1691,28 @@
         <v>2.0270193599999993</v>
       </c>
       <c r="J21" s="2">
+        <f t="shared" si="6"/>
+        <v>0.40775496524118782</v>
+      </c>
+      <c r="K21" s="2">
         <f t="shared" si="7"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K21" s="2">
-        <f t="shared" si="8"/>
         <v>2.4347743252411869</v>
       </c>
       <c r="L21" s="1"/>
-      <c r="M21">
+      <c r="M21" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="N21" s="32">
         <v>3</v>
       </c>
-      <c r="N21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="P21" s="35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
@@ -1531,40 +1732,43 @@
         <v>1</v>
       </c>
       <c r="G22" s="2">
+        <f t="shared" si="4"/>
+        <v>30.4</v>
+      </c>
+      <c r="H22" s="2">
         <f t="shared" si="5"/>
-        <v>30.4</v>
-      </c>
-      <c r="H22" s="2">
+        <v>0.56651008000000003</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="8"/>
+        <v>1.6995302400000001</v>
+      </c>
+      <c r="J22" s="2">
         <f t="shared" si="6"/>
-        <v>0.56651008000000003</v>
-      </c>
-      <c r="I22" s="2">
-        <f t="shared" si="9"/>
-        <v>1.6995302400000001</v>
-      </c>
-      <c r="J22" s="2">
+        <v>0.40775496524118782</v>
+      </c>
+      <c r="K22" s="2">
         <f t="shared" si="7"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K22" s="2">
-        <f t="shared" si="8"/>
         <v>2.1072852052411877</v>
       </c>
-      <c r="M22" s="25">
-        <f>M20*M21</f>
+      <c r="M22" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="N22" s="42">
+        <f>N20*N21</f>
         <v>1479</v>
       </c>
-      <c r="N22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="M24" s="23">
-        <f>M22+M19+M16</f>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M24" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="N24" s="44">
+        <f>N22+N19+N16</f>
         <v>4101.04</v>
       </c>
-      <c r="N24" s="23" t="s">
-        <v>43</v>
+      <c r="O24" s="35" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1610,20 +1814,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:10" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="6" t="s">
@@ -1698,7 +1902,7 @@
       <c r="B5" s="13">
         <v>2401.81</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="22">
         <v>0.875</v>
       </c>
       <c r="D5" s="16">
@@ -1725,7 +1929,7 @@
       <c r="B6" s="13">
         <v>1369</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="22">
         <v>0.875</v>
       </c>
       <c r="D6" s="16">
@@ -1750,7 +1954,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="13"/>
-      <c r="C7" s="27">
+      <c r="C7" s="22">
         <v>0.875</v>
       </c>
       <c r="D7" s="16"/>
@@ -1773,7 +1977,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="13"/>
-      <c r="C8" s="27">
+      <c r="C8" s="22">
         <v>0.875</v>
       </c>
       <c r="D8" s="16"/>
@@ -1796,7 +2000,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="13"/>
-      <c r="C9" s="27">
+      <c r="C9" s="22">
         <v>0.875</v>
       </c>
       <c r="D9" s="16"/>
@@ -1819,7 +2023,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="13"/>
-      <c r="C10" s="27">
+      <c r="C10" s="22">
         <v>0.875</v>
       </c>
       <c r="D10" s="16"/>
@@ -1842,7 +2046,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="13"/>
-      <c r="C11" s="27">
+      <c r="C11" s="22">
         <v>0.875</v>
       </c>
       <c r="D11" s="16"/>
@@ -1865,7 +2069,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="13"/>
-      <c r="C12" s="27">
+      <c r="C12" s="22">
         <v>0.875</v>
       </c>
       <c r="D12" s="16"/>
@@ -1888,7 +2092,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="13"/>
-      <c r="C13" s="27">
+      <c r="C13" s="22">
         <v>0.875</v>
       </c>
       <c r="D13" s="16"/>
@@ -1911,7 +2115,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="13"/>
-      <c r="C14" s="27">
+      <c r="C14" s="22">
         <v>0.875</v>
       </c>
       <c r="D14" s="16"/>
@@ -1929,17 +2133,17 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="I15" s="28">
+      <c r="I15" s="23">
         <f>F5</f>
         <v>3951.4519999999993</v>
       </c>
-      <c r="J15" s="28">
+      <c r="J15" s="23">
         <f>I15*2</f>
         <v>7902.9039999999986</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="J16" s="29">
+      <c r="J16" s="24">
         <f>J15/0.7</f>
         <v>11289.862857142856</v>
       </c>
@@ -1948,18 +2152,18 @@
       <c r="C17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="26" t="s">
-        <v>45</v>
+      <c r="D17" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="28">
+        <v>31</v>
+      </c>
+      <c r="J17" s="23">
         <f>J16/1000</f>
         <v>11.289862857142856</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
@@ -1974,15 +2178,15 @@
         <v>19.999999999999996</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>49</v>
+        <v>33</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alvenaria estrutural - definição dos carregamentos horizontais
</commit_message>
<xml_diff>
--- a/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
+++ b/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="83">
   <si>
     <t>Parede</t>
   </si>
@@ -166,9 +166,6 @@
     <t>Comprimento de parede</t>
   </si>
   <si>
-    <t>Tabela revit</t>
-  </si>
-  <si>
     <t>Comprimento por pavimento</t>
   </si>
   <si>
@@ -266,6 +263,12 @@
   </si>
   <si>
     <t>KN cal. lado</t>
+  </si>
+  <si>
+    <t>/ comprimento</t>
+  </si>
+  <si>
+    <t>Compimento total de paredes em metro. Tabela revit</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -542,6 +545,7 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,6 +589,7 @@
     <xf numFmtId="164" fontId="11" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Entrada" xfId="3" builtinId="20"/>
@@ -891,12 +896,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -905,7 +911,7 @@
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27" style="32" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27" style="33" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="46.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="61.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -954,7 +960,7 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="31" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="1"/>
@@ -1048,13 +1054,13 @@
         <f t="shared" ref="K6:K11" si="1">I6+J6</f>
         <v>1.6261591157689561</v>
       </c>
-      <c r="L6" s="31" t="s">
+      <c r="L6" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="M6" s="36" t="s">
+      <c r="M6" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="33">
+      <c r="N6" s="34">
         <v>18</v>
       </c>
     </row>
@@ -1098,7 +1104,7 @@
         <v>2.6864529557689565</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="37"/>
+      <c r="M7" s="38"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -1140,14 +1146,14 @@
         <v>2.6864529557689565</v>
       </c>
       <c r="L8" s="1"/>
-      <c r="M8" s="36" t="s">
+      <c r="M8" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="N8" s="34">
+      <c r="N8" s="35">
         <f>1/(100*SQRT(N6))</f>
         <v>2.3570226039551587E-3</v>
       </c>
-      <c r="O8" s="35" t="s">
+      <c r="O8" s="36" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1191,7 +1197,7 @@
         <v>2.4348777557689556</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="37"/>
+      <c r="M9" s="38"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -1233,14 +1239,14 @@
         <v>2.4348777557689556</v>
       </c>
       <c r="L10" s="1"/>
-      <c r="M10" s="36" t="s">
+      <c r="M10" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="32">
+      <c r="N10" s="33">
         <v>2423</v>
       </c>
-      <c r="O10" s="35" t="s">
-        <v>48</v>
+      <c r="O10" s="36" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1271,7 +1277,7 @@
         <v>0.56651008000000003</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="3"/>
+        <f>H11*3</f>
         <v>1.6995302400000001</v>
       </c>
       <c r="J11" s="2">
@@ -1283,15 +1289,15 @@
         <v>2.1073886357689564</v>
       </c>
       <c r="L11" s="1"/>
-      <c r="M11" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="N11" s="39">
+      <c r="M11" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="N11" s="40">
         <f>N10/6</f>
         <v>403.83333333333331</v>
       </c>
-      <c r="O11" s="35" t="s">
-        <v>50</v>
+      <c r="O11" s="36" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1308,19 +1314,19 @@
       <c r="I12" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="45" t="s">
-        <v>81</v>
+      <c r="J12" s="46" t="s">
+        <v>80</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="N12" s="32">
+      <c r="M12" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="N12" s="33">
         <v>2.8</v>
       </c>
-      <c r="O12" s="35" t="s">
-        <v>55</v>
+      <c r="O12" s="36" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1333,17 +1339,19 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="J13" s="47" t="s">
+        <v>81</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="N13" s="32">
+      <c r="M13" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="N13" s="33">
         <v>0.14000000000000001</v>
       </c>
-      <c r="O13" s="35" t="s">
-        <v>56</v>
+      <c r="O13" s="36" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1358,18 +1366,18 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="N14" s="32">
+      <c r="M14" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="N14" s="33">
         <v>15</v>
       </c>
-      <c r="O14" s="35" t="s">
-        <v>57</v>
+      <c r="O14" s="36" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="31" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="1"/>
@@ -1383,18 +1391,18 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="N15" s="39">
+      <c r="M15" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="N15" s="40">
         <f>N11*N12*N13</f>
         <v>158.30266666666665</v>
       </c>
-      <c r="O15" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="P15" s="35" t="s">
-        <v>77</v>
+      <c r="O15" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="P15" s="36" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1432,18 +1440,18 @@
         <v>37</v>
       </c>
       <c r="L16" s="1"/>
-      <c r="M16" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="N16" s="40">
+      <c r="M16" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="N16" s="41">
         <f>N14*N15</f>
         <v>2374.54</v>
       </c>
-      <c r="O16" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="P16" s="35" t="s">
-        <v>73</v>
+      <c r="O16" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="P16" s="36" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1478,25 +1486,25 @@
         <v>1.2183007199999998</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" ref="J17:J22" si="6">(4100*$N$8)/23.7</f>
-        <v>0.40775496524118782</v>
+        <f>(N24*$N$8)/29.1</f>
+        <v>0.33217333263657262</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" ref="K17:K22" si="7">I17+J17</f>
-        <v>1.6260556852411876</v>
+        <f t="shared" ref="K17:K22" si="6">I17+J17</f>
+        <v>1.5504740526365723</v>
       </c>
       <c r="L17" s="1"/>
-      <c r="M17" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="N17" s="32">
+      <c r="M17" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="N17" s="33">
         <v>99</v>
       </c>
-      <c r="O17" s="35" t="s">
+      <c r="O17" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="P17" s="36" t="s">
         <v>63</v>
-      </c>
-      <c r="P17" s="35" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -1531,25 +1539,25 @@
         <v>2.2785945600000002</v>
       </c>
       <c r="J18" s="2">
+        <f>(N24*$N$8)/29.1</f>
+        <v>0.33217333263657262</v>
+      </c>
+      <c r="K18" s="2">
         <f t="shared" si="6"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K18" s="2">
-        <f t="shared" si="7"/>
-        <v>2.6863495252411882</v>
+        <v>2.6107678926365727</v>
       </c>
       <c r="L18" s="1"/>
-      <c r="M18" s="36" t="s">
+      <c r="M18" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="N18" s="33">
+        <v>2.5</v>
+      </c>
+      <c r="O18" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="N18" s="32">
-        <v>2.5</v>
-      </c>
-      <c r="O18" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="P18" s="35" t="s">
-        <v>78</v>
+      <c r="P18" s="36" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -1580,30 +1588,30 @@
         <v>0.75953152000000013</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" ref="I19:I22" si="8">H19*3</f>
+        <f t="shared" ref="I19:I22" si="7">H19*3</f>
         <v>2.2785945600000002</v>
       </c>
       <c r="J19" s="2">
+        <f>(N24*$N$8)/29.1</f>
+        <v>0.33217333263657262</v>
+      </c>
+      <c r="K19" s="2">
         <f t="shared" si="6"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K19" s="2">
-        <f t="shared" si="7"/>
-        <v>2.6863495252411882</v>
+        <v>2.6107678926365727</v>
       </c>
       <c r="L19" s="1"/>
-      <c r="M19" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="N19" s="42">
+      <c r="M19" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N19" s="43">
         <f>N17*N18</f>
         <v>247.5</v>
       </c>
-      <c r="O19" s="35" t="s">
+      <c r="O19" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="P19" s="36" t="s">
         <v>71</v>
-      </c>
-      <c r="P19" s="35" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -1634,29 +1642,29 @@
         <v>0.67567311999999979</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2.0270193599999993</v>
       </c>
       <c r="J20" s="2">
+        <f>(N24*$N$8)/29.1</f>
+        <v>0.33217333263657262</v>
+      </c>
+      <c r="K20" s="2">
         <f t="shared" si="6"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K20" s="2">
-        <f t="shared" si="7"/>
-        <v>2.4347743252411869</v>
+        <v>2.3591926926365718</v>
       </c>
       <c r="L20" s="1"/>
-      <c r="M20" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="N20" s="32">
+      <c r="M20" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="N20" s="33">
         <v>493</v>
       </c>
-      <c r="O20" s="35" t="s">
+      <c r="O20" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="P20" s="36" t="s">
         <v>74</v>
-      </c>
-      <c r="P20" s="35" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -1691,25 +1699,25 @@
         <v>2.0270193599999993</v>
       </c>
       <c r="J21" s="2">
+        <f>(N24*$N$8)/29.1</f>
+        <v>0.33217333263657262</v>
+      </c>
+      <c r="K21" s="2">
         <f t="shared" si="6"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K21" s="2">
-        <f t="shared" si="7"/>
-        <v>2.4347743252411869</v>
+        <v>2.3591926926365718</v>
       </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="N21" s="32">
+      <c r="M21" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="N21" s="33">
         <v>3</v>
       </c>
-      <c r="O21" s="35" t="s">
+      <c r="O21" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="P21" s="36" t="s">
         <v>79</v>
-      </c>
-      <c r="P21" s="35" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -1740,35 +1748,35 @@
         <v>0.56651008000000003</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="8"/>
+        <f>H22*3</f>
         <v>1.6995302400000001</v>
       </c>
       <c r="J22" s="2">
+        <f>(N24*$N$8)/29.1</f>
+        <v>0.33217333263657262</v>
+      </c>
+      <c r="K22" s="2">
         <f t="shared" si="6"/>
-        <v>0.40775496524118782</v>
-      </c>
-      <c r="K22" s="2">
-        <f t="shared" si="7"/>
-        <v>2.1072852052411877</v>
-      </c>
-      <c r="M22" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="N22" s="42">
+        <v>2.0317035726365726</v>
+      </c>
+      <c r="M22" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="N22" s="43">
         <f>N20*N21</f>
         <v>1479</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M24" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="N24" s="44">
+      <c r="M24" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="N24" s="45">
         <f>N22+N19+N16</f>
         <v>4101.04</v>
       </c>
-      <c r="O24" s="35" t="s">
-        <v>76</v>
+      <c r="O24" s="36" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alvenaria estrutural - lançamento de carga peso próprio
</commit_message>
<xml_diff>
--- a/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
+++ b/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
@@ -477,7 +477,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -527,12 +527,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -590,6 +584,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Entrada" xfId="3" builtinId="20"/>
@@ -886,7 +889,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -896,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,44 +914,44 @@
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27" style="33" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27" style="31" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="46.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="61.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="27" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="1"/>
@@ -960,13 +963,13 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="27" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="1"/>
@@ -1011,7 +1014,7 @@
       <c r="K5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="25" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1050,17 +1053,17 @@
         <f>(N24*$N$8)/23.7</f>
         <v>0.40785839576895633</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="48">
         <f t="shared" ref="K6:K11" si="1">I6+J6</f>
         <v>1.6261591157689561</v>
       </c>
-      <c r="L6" s="32" t="s">
+      <c r="L6" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="M6" s="37" t="s">
+      <c r="M6" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="34">
+      <c r="N6" s="32">
         <v>18</v>
       </c>
     </row>
@@ -1088,7 +1091,7 @@
         <v>35.200000000000003</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" ref="H6:H11" si="2">(0.613*(G7^2))/1000</f>
+        <f t="shared" ref="H7:H11" si="2">(0.613*(G7^2))/1000</f>
         <v>0.75953152000000013</v>
       </c>
       <c r="I7" s="2">
@@ -1099,12 +1102,12 @@
         <f>(N24*N8)/23.7</f>
         <v>0.40785839576895633</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="48">
         <f t="shared" si="1"/>
         <v>2.6864529557689565</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="38"/>
+      <c r="M7" s="36"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -1134,26 +1137,26 @@
         <v>0.75953152000000013</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" ref="I8:I11" si="3">H8*3</f>
+        <f t="shared" ref="I8:I9" si="3">H8*3</f>
         <v>2.2785945600000002</v>
       </c>
       <c r="J8" s="2">
         <f>(N24*$N$8)/23.7</f>
         <v>0.40785839576895633</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="48">
         <f t="shared" si="1"/>
         <v>2.6864529557689565</v>
       </c>
       <c r="L8" s="1"/>
-      <c r="M8" s="37" t="s">
+      <c r="M8" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="N8" s="35">
+      <c r="N8" s="33">
         <f>1/(100*SQRT(N6))</f>
         <v>2.3570226039551587E-3</v>
       </c>
-      <c r="O8" s="36" t="s">
+      <c r="O8" s="34" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1192,12 +1195,12 @@
         <f>(N24*$N$8)/23.7</f>
         <v>0.40785839576895633</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="48">
         <f t="shared" si="1"/>
         <v>2.4348777557689556</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="38"/>
+      <c r="M9" s="36"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -1234,18 +1237,18 @@
         <f>(N24*$N$8)/23.7</f>
         <v>0.40785839576895633</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="48">
         <f t="shared" si="1"/>
         <v>2.4348777557689556</v>
       </c>
       <c r="L10" s="1"/>
-      <c r="M10" s="37" t="s">
+      <c r="M10" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="33">
+      <c r="N10" s="31">
         <v>2423</v>
       </c>
-      <c r="O10" s="36" t="s">
+      <c r="O10" s="34" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1284,19 +1287,19 @@
         <f>(N24*$N$8)/23.7</f>
         <v>0.40785839576895633</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="48">
         <f t="shared" si="1"/>
         <v>2.1073886357689564</v>
       </c>
       <c r="L11" s="1"/>
-      <c r="M11" s="39" t="s">
+      <c r="M11" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="N11" s="40">
+      <c r="N11" s="38">
         <f>N10/6</f>
         <v>403.83333333333331</v>
       </c>
-      <c r="O11" s="36" t="s">
+      <c r="O11" s="34" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1305,27 +1308,27 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="26" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="30" t="s">
+      <c r="I12" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="46" t="s">
+      <c r="J12" s="44" t="s">
         <v>80</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="37" t="s">
+      <c r="M12" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="N12" s="33">
+      <c r="N12" s="31">
         <v>2.8</v>
       </c>
-      <c r="O12" s="36" t="s">
+      <c r="O12" s="34" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1339,18 +1342,18 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="47" t="s">
+      <c r="J13" s="45" t="s">
         <v>81</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="37" t="s">
+      <c r="M13" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="N13" s="33">
+      <c r="N13" s="31">
         <v>0.14000000000000001</v>
       </c>
-      <c r="O13" s="36" t="s">
+      <c r="O13" s="34" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1366,18 +1369,18 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="37" t="s">
+      <c r="M14" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="N14" s="33">
+      <c r="N14" s="31">
         <v>15</v>
       </c>
-      <c r="O14" s="36" t="s">
+      <c r="O14" s="34" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="29" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="1"/>
@@ -1391,17 +1394,17 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="37" t="s">
+      <c r="M15" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="N15" s="40">
+      <c r="N15" s="38">
         <f>N11*N12*N13</f>
         <v>158.30266666666665</v>
       </c>
-      <c r="O15" s="36" t="s">
+      <c r="O15" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="P15" s="36" t="s">
+      <c r="P15" s="34" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1440,17 +1443,17 @@
         <v>37</v>
       </c>
       <c r="L16" s="1"/>
-      <c r="M16" s="42" t="s">
+      <c r="M16" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="N16" s="41">
+      <c r="N16" s="39">
         <f>N14*N15</f>
         <v>2374.54</v>
       </c>
-      <c r="O16" s="36" t="s">
+      <c r="O16" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="P16" s="36" t="s">
+      <c r="P16" s="34" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1489,21 +1492,21 @@
         <f>(N24*$N$8)/29.1</f>
         <v>0.33217333263657262</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="48">
         <f t="shared" ref="K17:K22" si="6">I17+J17</f>
         <v>1.5504740526365723</v>
       </c>
       <c r="L17" s="1"/>
-      <c r="M17" s="37" t="s">
+      <c r="M17" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="N17" s="33">
+      <c r="N17" s="31">
         <v>99</v>
       </c>
-      <c r="O17" s="36" t="s">
+      <c r="O17" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="P17" s="36" t="s">
+      <c r="P17" s="34" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1542,21 +1545,21 @@
         <f>(N24*$N$8)/29.1</f>
         <v>0.33217333263657262</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="48">
         <f t="shared" si="6"/>
         <v>2.6107678926365727</v>
       </c>
       <c r="L18" s="1"/>
-      <c r="M18" s="37" t="s">
+      <c r="M18" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="N18" s="33">
+      <c r="N18" s="31">
         <v>2.5</v>
       </c>
-      <c r="O18" s="36" t="s">
+      <c r="O18" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="P18" s="36" t="s">
+      <c r="P18" s="34" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1588,29 +1591,29 @@
         <v>0.75953152000000013</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" ref="I19:I22" si="7">H19*3</f>
+        <f t="shared" ref="I19:I20" si="7">H19*3</f>
         <v>2.2785945600000002</v>
       </c>
       <c r="J19" s="2">
         <f>(N24*$N$8)/29.1</f>
         <v>0.33217333263657262</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="48">
         <f t="shared" si="6"/>
         <v>2.6107678926365727</v>
       </c>
       <c r="L19" s="1"/>
-      <c r="M19" s="42" t="s">
+      <c r="M19" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="N19" s="43">
+      <c r="N19" s="41">
         <f>N17*N18</f>
         <v>247.5</v>
       </c>
-      <c r="O19" s="36" t="s">
+      <c r="O19" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="P19" s="36" t="s">
+      <c r="P19" s="34" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1649,21 +1652,21 @@
         <f>(N24*$N$8)/29.1</f>
         <v>0.33217333263657262</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="48">
         <f t="shared" si="6"/>
         <v>2.3591926926365718</v>
       </c>
       <c r="L20" s="1"/>
-      <c r="M20" s="37" t="s">
+      <c r="M20" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="N20" s="33">
+      <c r="N20" s="31">
         <v>493</v>
       </c>
-      <c r="O20" s="36" t="s">
+      <c r="O20" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="P20" s="36" t="s">
+      <c r="P20" s="34" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1702,21 +1705,21 @@
         <f>(N24*$N$8)/29.1</f>
         <v>0.33217333263657262</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="48">
         <f t="shared" si="6"/>
         <v>2.3591926926365718</v>
       </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="37" t="s">
+      <c r="M21" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="N21" s="33">
+      <c r="N21" s="31">
         <v>3</v>
       </c>
-      <c r="O21" s="36" t="s">
+      <c r="O21" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="P21" s="36" t="s">
+      <c r="P21" s="34" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1755,27 +1758,27 @@
         <f>(N24*$N$8)/29.1</f>
         <v>0.33217333263657262</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="48">
         <f t="shared" si="6"/>
         <v>2.0317035726365726</v>
       </c>
-      <c r="M22" s="42" t="s">
+      <c r="M22" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="N22" s="43">
+      <c r="N22" s="41">
         <f>N20*N21</f>
         <v>1479</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M24" s="44" t="s">
+      <c r="M24" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="N24" s="45">
+      <c r="N24" s="43">
         <f>N22+N19+N16</f>
         <v>4101.04</v>
       </c>
-      <c r="O24" s="36" t="s">
+      <c r="O24" s="34" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1822,15 +1825,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:10" thickTop="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
alvenaria estrutural - combinações de carga conforme NBR 15812 - parte 3
</commit_message>
<xml_diff>
--- a/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
+++ b/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="779"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="779" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tensões Vento e Desaprumo" sheetId="18" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="84">
   <si>
     <t>Parede</t>
   </si>
@@ -52,12 +52,6 @@
     <t>Vk (m/s)</t>
   </si>
   <si>
-    <t>he</t>
-  </si>
-  <si>
-    <t>te</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -124,15 +118,9 @@
     <t>fpk</t>
   </si>
   <si>
-    <t>= 2 x Tensão/0,70</t>
-  </si>
-  <si>
     <t>mpa</t>
   </si>
   <si>
-    <t>UTILIZAR BLOCOS DE 12 Mpa para o térreo</t>
-  </si>
-  <si>
     <t>Ft (kn/m)</t>
   </si>
   <si>
@@ -269,6 +257,42 @@
   </si>
   <si>
     <t>Compimento total de paredes em metro. Tabela revit</t>
+  </si>
+  <si>
+    <t>Altura efetiva (he)</t>
+  </si>
+  <si>
+    <t>Largura efetiva (te)</t>
+  </si>
+  <si>
+    <t>ABNT NBR 15812-1:2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 x Tensão/0,70</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UTILIZAR BLOCOS DE 12 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Mpa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> para o térreo</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -282,7 +306,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,6 +409,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -477,7 +521,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -486,47 +530,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -584,14 +595,92 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -889,7 +978,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -899,7 +988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -914,45 +1003,45 @@
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27" style="31" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27" style="14" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="46.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="61.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
+      <c r="A1" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="27" t="s">
-        <v>39</v>
+      <c r="E3" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -963,14 +1052,14 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>23</v>
+      <c r="A4" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="27" t="s">
-        <v>40</v>
+      <c r="E4" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -981,41 +1070,41 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="25" t="s">
-        <v>38</v>
+      <c r="I5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1053,17 +1142,17 @@
         <f>(N24*$N$8)/23.7</f>
         <v>0.40785839576895633</v>
       </c>
-      <c r="K6" s="48">
+      <c r="K6" s="29">
         <f t="shared" ref="K6:K11" si="1">I6+J6</f>
         <v>1.6261591157689561</v>
       </c>
-      <c r="L6" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="M6" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6" s="32">
+      <c r="L6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="15">
         <v>18</v>
       </c>
     </row>
@@ -1102,12 +1191,12 @@
         <f>(N24*N8)/23.7</f>
         <v>0.40785839576895633</v>
       </c>
-      <c r="K7" s="48">
+      <c r="K7" s="29">
         <f t="shared" si="1"/>
         <v>2.6864529557689565</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="36"/>
+      <c r="M7" s="19"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -1144,20 +1233,20 @@
         <f>(N24*$N$8)/23.7</f>
         <v>0.40785839576895633</v>
       </c>
-      <c r="K8" s="48">
+      <c r="K8" s="29">
         <f t="shared" si="1"/>
         <v>2.6864529557689565</v>
       </c>
       <c r="L8" s="1"/>
-      <c r="M8" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="N8" s="33">
+      <c r="M8" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="N8" s="16">
         <f>1/(100*SQRT(N6))</f>
         <v>2.3570226039551587E-3</v>
       </c>
-      <c r="O8" s="34" t="s">
-        <v>46</v>
+      <c r="O8" s="17" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1195,12 +1284,12 @@
         <f>(N24*$N$8)/23.7</f>
         <v>0.40785839576895633</v>
       </c>
-      <c r="K9" s="48">
+      <c r="K9" s="29">
         <f t="shared" si="1"/>
         <v>2.4348777557689556</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="36"/>
+      <c r="M9" s="19"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -1237,24 +1326,24 @@
         <f>(N24*$N$8)/23.7</f>
         <v>0.40785839576895633</v>
       </c>
-      <c r="K10" s="48">
+      <c r="K10" s="29">
         <f t="shared" si="1"/>
         <v>2.4348777557689556</v>
       </c>
       <c r="L10" s="1"/>
-      <c r="M10" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="N10" s="31">
+      <c r="M10" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="14">
         <v>2423</v>
       </c>
-      <c r="O10" s="34" t="s">
-        <v>82</v>
+      <c r="O10" s="17" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3">
         <v>3</v>
@@ -1287,20 +1376,20 @@
         <f>(N24*$N$8)/23.7</f>
         <v>0.40785839576895633</v>
       </c>
-      <c r="K11" s="48">
+      <c r="K11" s="29">
         <f t="shared" si="1"/>
         <v>2.1073886357689564</v>
       </c>
       <c r="L11" s="1"/>
-      <c r="M11" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="N11" s="38">
+      <c r="M11" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="N11" s="21">
         <f>N10/6</f>
         <v>403.83333333333331</v>
       </c>
-      <c r="O11" s="34" t="s">
-        <v>49</v>
+      <c r="O11" s="17" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1308,28 +1397,28 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="26" t="s">
-        <v>41</v>
+      <c r="E12" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="44" t="s">
-        <v>80</v>
+      <c r="I12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="35" t="s">
+      <c r="M12" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="N12" s="14">
+        <v>2.8</v>
+      </c>
+      <c r="O12" s="17" t="s">
         <v>50</v>
-      </c>
-      <c r="N12" s="31">
-        <v>2.8</v>
-      </c>
-      <c r="O12" s="34" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1342,19 +1431,19 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="45" t="s">
-        <v>81</v>
+      <c r="J13" s="28" t="s">
+        <v>77</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="35" t="s">
+      <c r="M13" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="N13" s="14">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O13" s="17" t="s">
         <v>51</v>
-      </c>
-      <c r="N13" s="31">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="O13" s="34" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1369,19 +1458,19 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="35" t="s">
+      <c r="M14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N14" s="14">
+        <v>15</v>
+      </c>
+      <c r="O14" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="N14" s="31">
-        <v>15</v>
-      </c>
-      <c r="O14" s="34" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
-        <v>24</v>
+      <c r="A15" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1394,67 +1483,67 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="N15" s="38">
+      <c r="M15" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="N15" s="21">
         <f>N11*N12*N13</f>
         <v>158.30266666666665</v>
       </c>
-      <c r="O15" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="P15" s="34" t="s">
-        <v>76</v>
+      <c r="O15" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="P15" s="17" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="20" t="s">
+      <c r="A16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="K16" s="20" t="s">
-        <v>37</v>
+      <c r="J16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="L16" s="1"/>
-      <c r="M16" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="N16" s="39">
+      <c r="M16" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" s="22">
         <f>N14*N15</f>
         <v>2374.54</v>
       </c>
-      <c r="O16" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="P16" s="34" t="s">
-        <v>72</v>
+      <c r="O16" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="P16" s="17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1492,22 +1581,22 @@
         <f>(N24*$N$8)/29.1</f>
         <v>0.33217333263657262</v>
       </c>
-      <c r="K17" s="48">
+      <c r="K17" s="29">
         <f t="shared" ref="K17:K22" si="6">I17+J17</f>
         <v>1.5504740526365723</v>
       </c>
       <c r="L17" s="1"/>
-      <c r="M17" s="35" t="s">
+      <c r="M17" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="N17" s="14">
+        <v>99</v>
+      </c>
+      <c r="O17" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="P17" s="17" t="s">
         <v>59</v>
-      </c>
-      <c r="N17" s="31">
-        <v>99</v>
-      </c>
-      <c r="O17" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="P17" s="34" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -1545,22 +1634,22 @@
         <f>(N24*$N$8)/29.1</f>
         <v>0.33217333263657262</v>
       </c>
-      <c r="K18" s="48">
+      <c r="K18" s="29">
         <f t="shared" si="6"/>
         <v>2.6107678926365727</v>
       </c>
       <c r="L18" s="1"/>
-      <c r="M18" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="N18" s="31">
+      <c r="M18" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="N18" s="14">
         <v>2.5</v>
       </c>
-      <c r="O18" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="P18" s="34" t="s">
-        <v>77</v>
+      <c r="O18" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="P18" s="17" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -1598,23 +1687,23 @@
         <f>(N24*$N$8)/29.1</f>
         <v>0.33217333263657262</v>
       </c>
-      <c r="K19" s="48">
+      <c r="K19" s="29">
         <f t="shared" si="6"/>
         <v>2.6107678926365727</v>
       </c>
       <c r="L19" s="1"/>
-      <c r="M19" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="N19" s="41">
+      <c r="M19" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="N19" s="24">
         <f>N17*N18</f>
         <v>247.5</v>
       </c>
-      <c r="O19" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="P19" s="34" t="s">
-        <v>71</v>
+      <c r="O19" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="P19" s="17" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -1652,22 +1741,22 @@
         <f>(N24*$N$8)/29.1</f>
         <v>0.33217333263657262</v>
       </c>
-      <c r="K20" s="48">
+      <c r="K20" s="29">
         <f t="shared" si="6"/>
         <v>2.3591926926365718</v>
       </c>
       <c r="L20" s="1"/>
-      <c r="M20" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="N20" s="31">
+      <c r="M20" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="N20" s="14">
         <v>493</v>
       </c>
-      <c r="O20" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="P20" s="34" t="s">
-        <v>74</v>
+      <c r="O20" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="P20" s="17" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -1705,27 +1794,27 @@
         <f>(N24*$N$8)/29.1</f>
         <v>0.33217333263657262</v>
       </c>
-      <c r="K21" s="48">
+      <c r="K21" s="29">
         <f t="shared" si="6"/>
         <v>2.3591926926365718</v>
       </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="N21" s="31">
+      <c r="M21" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="N21" s="14">
         <v>3</v>
       </c>
-      <c r="O21" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="P21" s="34" t="s">
-        <v>79</v>
+      <c r="O21" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="P21" s="17" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3">
         <v>3</v>
@@ -1758,28 +1847,28 @@
         <f>(N24*$N$8)/29.1</f>
         <v>0.33217333263657262</v>
       </c>
-      <c r="K22" s="48">
+      <c r="K22" s="29">
         <f t="shared" si="6"/>
         <v>2.0317035726365726</v>
       </c>
-      <c r="M22" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="N22" s="41">
+      <c r="M22" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="N22" s="24">
         <f>N20*N21</f>
         <v>1479</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M24" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="N24" s="43">
+      <c r="M24" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="N24" s="26">
         <f>N22+N19+N16</f>
         <v>4101.04</v>
       </c>
-      <c r="O24" s="34" t="s">
-        <v>75</v>
+      <c r="O24" s="17" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1793,412 +1882,509 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" style="17" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="6"/>
-    <col min="9" max="9" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" style="6" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="23.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="2" spans="1:10" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="6">
+    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="32">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="6">
+      <c r="E2" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="32">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="11">
+      <c r="G2" s="34"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="34">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="11">
+      <c r="C3" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="34">
         <v>2.8</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="6">
+      <c r="E3" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="32">
         <f>D3/B3</f>
         <v>19.999999999999996</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="7"/>
-      <c r="J3" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="G3" s="36"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="56" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="F4" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="19">
-        <v>1</v>
-      </c>
-      <c r="B5" s="13">
+      <c r="G4" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="32"/>
+      <c r="I4" s="56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="41">
+        <v>1</v>
+      </c>
+      <c r="B5" s="42">
         <v>2401.81</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="43">
         <v>0.875</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="44">
         <v>116.31</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="45">
         <f>(B5/C5)+(D5/1.5)</f>
         <v>2822.4657142857141</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="46">
         <f t="shared" ref="F5:F14" si="0">E5*1.4</f>
         <v>3951.4519999999993</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="45">
         <f>-(B5*0.9)+(D5*1.4)</f>
         <v>-1998.7949999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="19">
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="41">
         <f>A5+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="42">
         <v>1369</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="43">
         <v>0.875</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="44">
         <v>104.58</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="45">
         <f t="shared" ref="E6:E14" si="1">(B6/C6)+(D6/1.5)</f>
         <v>1634.2914285714287</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="46">
         <f t="shared" si="0"/>
         <v>2288.0079999999998</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="45">
         <f>-(B6*0.9)+(D6*1.4)</f>
         <v>-1085.6880000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="19">
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="41">
         <f t="shared" ref="A7:A14" si="2">A6+1</f>
         <v>3</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="22">
+      <c r="B7" s="42"/>
+      <c r="C7" s="43">
         <v>0.875</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="12">
+      <c r="D7" s="44"/>
+      <c r="E7" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="45">
         <f t="shared" ref="G7:G14" si="3">-(B7*0.9)+(D7*1.4)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="19">
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="41">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="22">
+      <c r="B8" s="42"/>
+      <c r="C8" s="43">
         <v>0.875</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="12">
+      <c r="D8" s="44"/>
+      <c r="E8" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="19">
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="41">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="22">
+      <c r="B9" s="42"/>
+      <c r="C9" s="43">
         <v>0.875</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="12">
+      <c r="D9" s="44"/>
+      <c r="E9" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="19">
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="41">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="22">
+      <c r="B10" s="42"/>
+      <c r="C10" s="43">
         <v>0.875</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="12">
+      <c r="D10" s="44"/>
+      <c r="E10" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="19">
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="41">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="22">
+      <c r="B11" s="42"/>
+      <c r="C11" s="43">
         <v>0.875</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="12">
+      <c r="D11" s="44"/>
+      <c r="E11" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="19">
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="41">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="22">
+      <c r="B12" s="42"/>
+      <c r="C12" s="43">
         <v>0.875</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="12">
+      <c r="D12" s="44"/>
+      <c r="E12" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="19">
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="41">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="22">
+      <c r="B13" s="42"/>
+      <c r="C13" s="43">
         <v>0.875</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="12">
+      <c r="D13" s="44"/>
+      <c r="E13" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="19">
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="41">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="22">
+      <c r="B14" s="42"/>
+      <c r="C14" s="43">
         <v>0.875</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="12">
+      <c r="D14" s="44"/>
+      <c r="E14" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="I15" s="23">
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="35"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="47">
         <f>F5</f>
         <v>3951.4519999999993</v>
       </c>
-      <c r="J15" s="23">
-        <f>I15*2</f>
+      <c r="I15" s="47">
+        <f>H15*2</f>
         <v>7902.9039999999986</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="J16" s="24">
-        <f>J15/0.7</f>
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="35"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="48">
+        <f>I15/0.7</f>
         <v>11289.862857142856</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="C17" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" s="23">
-        <f>J16/1000</f>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="35"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="32"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="47">
+        <f>I16/1000</f>
         <v>11.289862857142856</v>
       </c>
-      <c r="K17" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="E18" s="6">
+      <c r="J17" s="57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="35"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="54">
         <f>1-(20/40)^3</f>
         <v>0.875</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D20" s="6">
-        <f>2.8/0.14</f>
-        <v>19.999999999999996</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>34</v>
-      </c>
+      <c r="F18" s="32"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="35"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="35"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="35"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="32"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="35"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2215,6 +2401,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
alvenaria estrutural - análise estrutural na nuvem
</commit_message>
<xml_diff>
--- a/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
+++ b/revit_alvenaria_estrutural/Tabela de pré dimensionamento blocos estruturais.xlsx
@@ -521,7 +521,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -681,6 +681,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1885,7 +1888,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2258,7 +2261,7 @@
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="35"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
@@ -2266,7 +2269,7 @@
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>
       <c r="G15" s="34"/>
-      <c r="H15" s="47">
+      <c r="H15" s="58">
         <f>F5</f>
         <v>3951.4519999999993</v>
       </c>

</xml_diff>